<commit_message>
fixes small buggs and add statistics functions
</commit_message>
<xml_diff>
--- a/data-raw/8f_cost_burden_disease.xlsx
+++ b/data-raw/8f_cost_burden_disease.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339A7159-058A-364A-8196-D9A4FFC4B78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD2D3FD-9E43-7A49-B403-EA4777A35501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D87C1428-1815-D049-A73F-EF0C17CE80CD}"/>
+    <workbookView xWindow="30400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D87C1428-1815-D049-A73F-EF0C17CE80CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,8 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00_-\ [$€-1];[Red]#,##0.00\-\ [$€-1]"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -150,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -162,9 +161,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -487,7 +483,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -500,7 +496,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -556,59 +552,59 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5">
-        <v>95.295690000000008</v>
-      </c>
-      <c r="C2" s="5">
-        <v>325.69166666666666</v>
-      </c>
-      <c r="D2" s="5">
-        <v>579.27800000000002</v>
-      </c>
-      <c r="E2" s="5">
-        <v>105.7085</v>
-      </c>
-      <c r="F2" s="5">
-        <v>186.23083030198185</v>
-      </c>
-      <c r="G2" s="5">
-        <v>121.57738309458219</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2870.7933333333331</v>
-      </c>
-      <c r="I2" s="5">
-        <v>2019.6</v>
-      </c>
-      <c r="J2" s="5">
-        <v>167.19332373294768</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="B2" s="1">
+        <v>102.89816838000002</v>
+      </c>
+      <c r="C2" s="1">
+        <v>302.17330000000004</v>
+      </c>
+      <c r="D2">
+        <v>448.85769599999998</v>
+      </c>
+      <c r="E2">
+        <v>86.004435599999994</v>
+      </c>
+      <c r="F2">
+        <v>103.16822442029093</v>
+      </c>
+      <c r="G2">
+        <v>117.75637962589533</v>
+      </c>
+      <c r="H2">
+        <v>1673.2624000000001</v>
+      </c>
+      <c r="I2">
+        <v>1156.2883199999999</v>
+      </c>
+      <c r="J2">
+        <v>195.33871899624728</v>
+      </c>
+      <c r="K2">
         <v>15.66</v>
       </c>
-      <c r="L2" s="5">
-        <v>14.195999999999998</v>
-      </c>
-      <c r="M2" s="5">
-        <v>2.879</v>
-      </c>
-      <c r="N2" s="5">
-        <v>847.32853333333333</v>
-      </c>
-      <c r="O2" s="5">
-        <v>141.43866666666668</v>
-      </c>
-      <c r="P2" s="5">
-        <v>784.93133333333333</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>159.58693333333335</v>
-      </c>
-      <c r="R2" s="5">
-        <v>10062.020867460158</v>
+      <c r="L2">
+        <v>24.189983999999999</v>
+      </c>
+      <c r="M2">
+        <v>1.951962</v>
+      </c>
+      <c r="N2">
+        <v>587.42976319999991</v>
+      </c>
+      <c r="O2">
+        <v>76.716332800000004</v>
+      </c>
+      <c r="P2">
+        <v>475.56818399999997</v>
+      </c>
+      <c r="Q2">
+        <v>152.5275584</v>
+      </c>
+      <c r="R2">
+        <v>7630.3786967924143</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update and finalise all plots based on feedback meeting
</commit_message>
<xml_diff>
--- a/data-raw/8f_cost_burden_disease.xlsx
+++ b/data-raw/8f_cost_burden_disease.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675E6842-E0C9-2244-A6D4-F4F5E69EBF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01F1AC5-8807-854B-8CD0-A94211CF7C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D87C1428-1815-D049-A73F-EF0C17CE80CD}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="21780" windowHeight="17500" xr2:uid="{D87C1428-1815-D049-A73F-EF0C17CE80CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>inpatient_services</t>
   </si>
@@ -59,40 +59,43 @@
     <t>vision_aids</t>
   </si>
   <si>
+    <t>home_care_household</t>
+  </si>
+  <si>
+    <t>home_care_personal</t>
+  </si>
+  <si>
+    <t>informal_care_household</t>
+  </si>
+  <si>
+    <t>informal_care_personal</t>
+  </si>
+  <si>
+    <t>informal_care_communication</t>
+  </si>
+  <si>
+    <t>informal_care_companionship</t>
+  </si>
+  <si>
+    <t>productivity_absent</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>vi_sev</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>transportation</t>
   </si>
   <si>
-    <t>home_care_household</t>
-  </si>
-  <si>
-    <t>home_care_personal</t>
-  </si>
-  <si>
-    <t>informal_care_household</t>
-  </si>
-  <si>
-    <t>informal_care_personal</t>
-  </si>
-  <si>
-    <t>informal_care_communication</t>
-  </si>
-  <si>
-    <t>informal_care_companionship</t>
-  </si>
-  <si>
-    <t>productivity_absent</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>vi_sev</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>general_practitioner</t>
+    <t>measuring_devices</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2D911C-B066-4D4D-B60E-45CA815F5FC1}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -492,18 +495,18 @@
     <col min="2" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -527,33 +530,36 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>102.89816838000002</v>
@@ -583,34 +589,37 @@
         <v>195.33871899624728</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>15.66</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>24.189983999999999</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1.951962</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>587.42976319999991</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>76.716332800000004</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>475.56818399999997</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>152.5275584</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>7630.3786967924143</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>

</xml_diff>